<commit_message>
Tracking user actions with Cookies
</commit_message>
<xml_diff>
--- a/me_docs/4.State-Management-with-JSP.xlsx
+++ b/me_docs/4.State-Management-with-JSP.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F16C02-8AA2-4DC0-9634-E59CA4B460DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB844F9-5414-4221-9986-6BBA1B4FF8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Cookies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Create todo-demo.jsp</t>
   </si>
   <si>
     <t>Check by browser</t>
+  </si>
+  <si>
+    <t>Create cookies-personalize-form.html</t>
+  </si>
+  <si>
+    <t>Create cookies-personalize-response.jsp</t>
+  </si>
+  <si>
+    <t>Create cookies-homepage.jsp</t>
   </si>
 </sst>
 </file>
@@ -387,6 +397,627 @@
         <a:xfrm>
           <a:off x="609600" y="24765000"/>
           <a:ext cx="4895238" cy="2085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65828</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C35776B-3BD0-4D51-B3C5-E87304DC91C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6771428" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>151690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA0E0FEB-0324-4766-9862-D0AEA1AC7F93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5334000"/>
+          <a:ext cx="4866667" cy="5676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>503924</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>47071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25755436-A484-4E36-B230-CADDD942272A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11239500"/>
+          <a:ext cx="7209524" cy="4428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65828</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>180381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25285CC5-B63C-40D5-9B18-9AAFC20D2E4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16192500"/>
+          <a:ext cx="6771428" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>180262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA247689-0E8F-478C-B776-BD8C8CCEC36F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="21145500"/>
+          <a:ext cx="4866667" cy="5704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>608533</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>75476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DF638FD-5FC3-4A42-BBE4-18554367E131}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="27051000"/>
+          <a:ext cx="8533333" cy="5790476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65828</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>180381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3269A0C-144C-4A62-B438-B1F77FFAE9F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="33337500"/>
+          <a:ext cx="6771428" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>589943</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>151690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43976444-2D72-4631-94B6-1ABDB38AAD67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="38290500"/>
+          <a:ext cx="4857143" cy="5676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>8457</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>18286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D51F6A-EAE2-4B04-8527-58222459E2E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="44196000"/>
+          <a:ext cx="8542857" cy="6114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>132724</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>37548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F644CFCE-F038-4061-83D5-F354161DCF01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="50863500"/>
+          <a:ext cx="5009524" cy="4419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>292</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18438</xdr:colOff>
+      <xdr:row>300</xdr:row>
+      <xdr:rowOff>47429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F28D91A8-21A9-4E5F-BCCD-94DFD369C547}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="55626000"/>
+          <a:ext cx="4895238" cy="1571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>302</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46781</xdr:colOff>
+      <xdr:row>310</xdr:row>
+      <xdr:rowOff>171238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82558BB2-4BFC-47C1-A79A-E8D77B707928}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="57531000"/>
+          <a:ext cx="6752381" cy="1695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>313</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>37486</xdr:colOff>
+      <xdr:row>336</xdr:row>
+      <xdr:rowOff>18500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22BBF396-6AED-45ED-B475-AE3506F0499D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="59626500"/>
+          <a:ext cx="4914286" cy="4400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>338</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>198400</xdr:colOff>
+      <xdr:row>353</xdr:row>
+      <xdr:rowOff>132976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8907E1EA-C90A-4AF8-A730-771B67C80F8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="64389000"/>
+          <a:ext cx="13000000" cy="2990476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -664,8 +1295,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:A96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,4 +1316,40 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AA8CAA-A6C6-43F3-BA07-A711A339BA05}">
+  <dimension ref="A2:A267"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
+      <selection activeCell="Q336" sqref="Q336"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>